<commit_message>
segmentando la app por proyecto 1
</commit_message>
<xml_diff>
--- a/static/Technician_Prices_Template.xlsx
+++ b/static/Technician_Prices_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisg\OneDrive\Escritorio\APP\hyperlink_networks\hyperlink_networks\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisenriquegilmoya/Desktop/APP/hyperlink_networks/staticfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D741AC55-2BFE-463F-9B66-26B2E0078FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CAEC60-5427-9F48-847D-C151FF814F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10800" xr2:uid="{EC3D08FF-665D-41CD-8D67-D677F48A1D49}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20500" windowHeight="10800" xr2:uid="{EC3D08FF-665D-41CD-8D67-D677F48A1D49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>City</t>
   </si>
   <si>
-    <t>Proyect</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -64,6 +61,27 @@
   </si>
   <si>
     <t>Office</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>CCU</t>
+  </si>
+  <si>
+    <t>Fiber</t>
+  </si>
+  <si>
+    <t>j123</t>
+  </si>
+  <si>
+    <t>Nodo</t>
+  </si>
+  <si>
+    <t>un</t>
   </si>
 </sst>
 </file>
@@ -139,7 +157,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -168,9 +186,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +226,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -314,7 +332,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,7 +474,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -464,35 +482,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC3FA0B-DC05-4AAA-87A7-04EC1BFAD17B}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -501,7 +518,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -512,23 +529,37 @@
       <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -538,9 +569,8 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -550,9 +580,8 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -562,9 +591,8 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -574,9 +602,8 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -586,9 +613,8 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -598,9 +624,8 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -610,9 +635,8 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -622,9 +646,8 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -634,9 +657,8 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -646,9 +668,8 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -658,9 +679,8 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -670,9 +690,8 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -682,9 +701,8 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -694,9 +712,8 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -706,9 +723,8 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -718,9 +734,8 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -730,9 +745,8 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -742,9 +756,8 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -754,9 +767,8 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -766,9 +778,8 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -778,9 +789,8 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -790,9 +800,8 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -802,7 +811,6 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>